<commit_message>
Modify postal excel file and util.py for testing; added test cases for property and taxlot postal code.
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-postal.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-postal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E66AE7-3524-1243-9E0C-795C8B4D01F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761DD01B-22CE-284D-B228-A678603F2BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38560" yWindow="2000" windowWidth="38400" windowHeight="19640" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="122">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -384,10 +384,16 @@
     <t>12345-6789</t>
   </si>
   <si>
-    <t>zip fake</t>
-  </si>
-  <si>
     <t>1-2</t>
+  </si>
+  <si>
+    <t>postal code</t>
+  </si>
+  <si>
+    <t>93030 Wellington Blvd</t>
+  </si>
+  <si>
+    <t>address</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -453,6 +459,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1050,10 +1062,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1064,27 +1076,27 @@
     <col min="4" max="4" width="14" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.83203125" style="12"/>
-    <col min="21" max="21" width="12.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.83203125" style="12"/>
+    <col min="7" max="8" width="18.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="39.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="8.83203125" style="12"/>
+    <col min="22" max="22" width="12.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>95</v>
       </c>
@@ -1107,64 +1119,67 @@
         <v>83</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>118</v>
+      <c r="AA1" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5">
         <v>1</v>
       </c>
@@ -1182,64 +1197,67 @@
         <v>2</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>1552813</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>75</v>
       </c>
-      <c r="L2" s="7">
+      <c r="M2" s="7">
         <v>125</v>
       </c>
-      <c r="M2" s="8">
+      <c r="N2" s="8">
         <v>42369</v>
       </c>
-      <c r="N2" s="9">
+      <c r="O2" s="9">
         <v>12555</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="5">
+      <c r="T2" s="5">
         <v>39.755543000000003</v>
       </c>
-      <c r="T2" s="5">
+      <c r="U2" s="5">
         <v>-105.22110000000001</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="V2" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="25">
+      <c r="W2" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W2" s="25">
+      <c r="X2" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="Z2" s="7">
         <v>1</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="AA2" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5">
         <v>4</v>
       </c>
@@ -1257,64 +1275,67 @@
         <v>77</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="7">
         <v>11160509</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="7">
         <v>63</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>1202</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="8">
         <v>42369</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <v>23543</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="5">
+      <c r="T3" s="5">
         <v>39.751511000000001</v>
       </c>
-      <c r="T3" s="5">
+      <c r="U3" s="5">
         <v>-105.225381</v>
       </c>
-      <c r="U3" s="24">
+      <c r="V3" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V3" s="25">
+      <c r="W3" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W3" s="25">
+      <c r="X3" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="Y3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="Y3" s="7">
+      <c r="Z3" s="7">
         <v>4</v>
       </c>
-      <c r="Z3" s="28" t="s">
-        <v>119</v>
+      <c r="AA3" s="28" t="s">
+        <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>6</v>
       </c>
@@ -1334,62 +1355,65 @@
         <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="7">
         <v>24651456</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="8">
         <v>42369</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="R4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="5">
+      <c r="T4" s="5">
         <v>39.740510999999998</v>
       </c>
-      <c r="T4" s="5">
+      <c r="U4" s="5">
         <v>-105.17121</v>
       </c>
-      <c r="U4" s="24"/>
-      <c r="V4" s="25">
+      <c r="V4" s="24"/>
+      <c r="W4" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W4" s="25">
+      <c r="X4" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="Y4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Z4" s="7">
         <v>6</v>
       </c>
-      <c r="Z4" s="27">
-        <v>34</v>
+      <c r="AA4" s="27">
+        <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>7</v>
       </c>
@@ -1409,64 +1433,67 @@
         <v>50</v>
       </c>
       <c r="H5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>24651456</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>77</v>
       </c>
-      <c r="L5" s="7">
+      <c r="M5" s="7">
         <v>219</v>
       </c>
-      <c r="M5" s="8">
+      <c r="N5" s="8">
         <v>42369</v>
       </c>
-      <c r="N5" s="13">
+      <c r="O5" s="13">
         <v>124523</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="R5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S5" s="5">
+      <c r="T5" s="5">
         <v>39.734164</v>
       </c>
-      <c r="T5" s="5">
+      <c r="U5" s="5">
         <v>-105.159808</v>
       </c>
-      <c r="U5" s="24">
+      <c r="V5" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V5" s="25">
+      <c r="W5" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W5" s="25">
+      <c r="X5" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Z5" s="7">
         <v>7</v>
       </c>
-      <c r="Z5" s="27">
+      <c r="AA5" s="27">
         <v>88051</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>11</v>
       </c>
@@ -1486,64 +1513,67 @@
         <v>49</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="7">
         <v>24651456</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="7">
+      <c r="L6" s="7">
         <v>43</v>
       </c>
-      <c r="L6" s="7">
+      <c r="M6" s="7">
         <v>84</v>
       </c>
-      <c r="M6" s="8">
+      <c r="N6" s="8">
         <v>42369</v>
       </c>
-      <c r="N6" s="13">
+      <c r="O6" s="13">
         <v>421351</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="5">
+      <c r="T6" s="5">
         <v>39.733597000000003</v>
       </c>
-      <c r="T6" s="5">
+      <c r="U6" s="5">
         <v>-105.162576</v>
       </c>
-      <c r="U6" s="24">
+      <c r="V6" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V6" s="25">
+      <c r="W6" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W6" s="25">
+      <c r="X6" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Z6" s="7">
         <v>8</v>
       </c>
-      <c r="Z6" s="27">
+      <c r="AA6" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5">
         <v>8</v>
@@ -1564,64 +1594,67 @@
         <v>51</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>24651456</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="7">
+      <c r="L7" s="7">
         <v>59</v>
       </c>
-      <c r="L7" s="7">
+      <c r="M7" s="7">
         <v>72</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>42369</v>
       </c>
-      <c r="N7" s="13">
+      <c r="O7" s="13">
         <v>1234</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="P7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="Q7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="R7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="S7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S7" s="12">
+      <c r="T7" s="12">
         <v>39.739111000000001</v>
       </c>
-      <c r="T7" s="12">
+      <c r="U7" s="12">
         <v>-104.984951</v>
       </c>
-      <c r="U7" s="24">
+      <c r="V7" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V7" s="25">
+      <c r="W7" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W7" s="25">
+      <c r="X7" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X7" s="9" t="s">
+      <c r="Y7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Z7" s="7">
         <v>9</v>
       </c>
-      <c r="Z7" s="27">
+      <c r="AA7" s="27">
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5">
         <v>9</v>
@@ -1642,64 +1675,67 @@
         <v>24</v>
       </c>
       <c r="H8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="7">
+      <c r="L8" s="7">
         <v>34</v>
       </c>
-      <c r="L8" s="7">
+      <c r="M8" s="7">
         <v>45</v>
       </c>
-      <c r="M8" s="8">
+      <c r="N8" s="8">
         <v>42369</v>
       </c>
-      <c r="N8" s="13">
+      <c r="O8" s="13">
         <v>45324</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="Q8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q8" s="11" t="s">
+      <c r="R8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="S8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="12">
+      <c r="T8" s="12">
         <v>39.731361</v>
       </c>
-      <c r="T8" s="12">
+      <c r="U8" s="12">
         <v>-104.96074299999999</v>
       </c>
-      <c r="U8" s="24">
+      <c r="V8" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V8" s="25">
+      <c r="W8" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W8" s="25">
+      <c r="X8" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X8" s="9" t="s">
+      <c r="Y8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Z8" s="7">
         <v>10</v>
       </c>
-      <c r="Z8" s="27" t="s">
+      <c r="AA8" s="27" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5">
         <v>12</v>
@@ -1717,67 +1753,70 @@
         <v>23</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="H9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="8">
         <v>42369</v>
       </c>
-      <c r="N9" s="13">
+      <c r="O9" s="13">
         <v>482215</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="P9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="Q9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="11" t="s">
+      <c r="R9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="S9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S9" s="12">
+      <c r="T9" s="12">
         <v>39.741906999999998</v>
       </c>
-      <c r="T9" s="12">
+      <c r="U9" s="12">
         <v>-104.975129</v>
       </c>
-      <c r="U9" s="24">
+      <c r="V9" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V9" s="25">
+      <c r="W9" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W9" s="25">
+      <c r="X9" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X9" s="9" t="s">
+      <c r="Y9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Z9" s="7">
         <v>11</v>
       </c>
-      <c r="Z9" s="27">
+      <c r="AA9" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5">
         <v>2</v>
@@ -1796,64 +1835,67 @@
         <v>4</v>
       </c>
       <c r="H10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
         <v>11160509</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="7">
+      <c r="L10" s="7">
         <v>1</v>
       </c>
-      <c r="L10" s="7">
+      <c r="M10" s="7">
         <v>652.29999999999995</v>
       </c>
-      <c r="M10" s="8">
+      <c r="N10" s="8">
         <v>42369</v>
       </c>
-      <c r="N10" s="9">
+      <c r="O10" s="9">
         <v>513852</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="R10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="S10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S10" s="12">
+      <c r="T10" s="12">
         <v>39.742130000000003</v>
       </c>
-      <c r="T10" s="12">
+      <c r="U10" s="12">
         <v>-104.996673</v>
       </c>
-      <c r="U10" s="24">
+      <c r="V10" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V10" s="25">
+      <c r="W10" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W10" s="25">
+      <c r="X10" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X10" s="9" t="s">
+      <c r="Y10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Z10" s="7">
         <v>2</v>
       </c>
-      <c r="Z10" s="27">
+      <c r="AA10" s="27">
         <v>80504</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5">
         <v>3</v>
@@ -1872,64 +1914,67 @@
         <v>5</v>
       </c>
       <c r="H11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>11160509</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="8">
         <v>42369</v>
       </c>
-      <c r="N11" s="9">
+      <c r="O11" s="9">
         <v>55121</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="P11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="Q11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="R11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="S11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S11" s="12">
+      <c r="T11" s="12">
         <v>40.014986</v>
       </c>
-      <c r="T11" s="12">
+      <c r="U11" s="12">
         <v>-105.270546</v>
       </c>
-      <c r="U11" s="24">
+      <c r="V11" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V11" s="25">
+      <c r="W11" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W11" s="25">
+      <c r="X11" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X11" s="9" t="s">
+      <c r="Y11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Z11" s="7">
         <v>3</v>
       </c>
-      <c r="Z11" s="27">
+      <c r="AA11" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -1948,64 +1993,67 @@
         <v>0</v>
       </c>
       <c r="H12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="K12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="7">
+      <c r="L12" s="7">
         <v>55</v>
       </c>
-      <c r="L12" s="7">
+      <c r="M12" s="7">
         <v>1358</v>
       </c>
-      <c r="M12" s="8">
+      <c r="N12" s="8">
         <v>42369</v>
       </c>
-      <c r="N12" s="9">
+      <c r="O12" s="9">
         <v>200000</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="Q12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="R12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="7" t="s">
+      <c r="S12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S12" s="12">
+      <c r="T12" s="12">
         <v>40.007199</v>
       </c>
-      <c r="T12" s="12">
+      <c r="U12" s="12">
         <v>-105.26486800000001</v>
       </c>
-      <c r="U12" s="24">
+      <c r="V12" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V12" s="25">
+      <c r="W12" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W12" s="25">
+      <c r="X12" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X12" s="9" t="s">
+      <c r="Y12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="Z12" s="7">
         <v>5</v>
       </c>
-      <c r="Z12" s="27">
+      <c r="AA12" s="27">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>10</v>
       </c>
@@ -2022,64 +2070,67 @@
         <v>52</v>
       </c>
       <c r="H13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="16">
+      <c r="J13" s="16">
         <v>13334485</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="K13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="7">
+      <c r="L13" s="7">
         <v>88</v>
       </c>
-      <c r="L13" s="7">
+      <c r="M13" s="7">
         <v>942</v>
       </c>
-      <c r="M13" s="8">
+      <c r="N13" s="8">
         <v>42369</v>
       </c>
-      <c r="N13" s="14">
+      <c r="O13" s="14">
         <v>24523</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="P13" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="Q13" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="Q13" s="15" t="s">
+      <c r="R13" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R13" s="7" t="s">
+      <c r="S13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="S13" s="12">
+      <c r="T13" s="12">
         <v>39.999355999999999</v>
       </c>
-      <c r="T13" s="12">
+      <c r="U13" s="12">
         <v>-105.26242000000001</v>
       </c>
-      <c r="U13" s="24">
+      <c r="V13" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V13" s="25">
+      <c r="W13" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W13" s="25">
+      <c r="X13" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X13" s="9" t="s">
+      <c r="Y13" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="Z13" s="7">
         <v>12</v>
       </c>
-      <c r="Z13" s="27">
+      <c r="AA13" s="27">
         <v>13089</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17">
         <v>13</v>
@@ -2098,64 +2149,67 @@
         <v>74</v>
       </c>
       <c r="H14" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="17">
+      <c r="J14" s="17">
         <v>1234</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="K14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="18">
+      <c r="L14" s="18">
         <v>34</v>
       </c>
-      <c r="L14" s="18">
+      <c r="M14" s="18">
         <v>45</v>
       </c>
-      <c r="M14" s="19">
+      <c r="N14" s="19">
         <v>42369</v>
       </c>
-      <c r="N14" s="20">
+      <c r="O14" s="20">
         <v>45324</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="P14" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="17" t="s">
+      <c r="Q14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Q14" s="21" t="s">
+      <c r="R14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="R14" s="17" t="s">
+      <c r="S14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="S14" s="12">
+      <c r="T14" s="12">
         <v>39.74389</v>
       </c>
-      <c r="T14" s="12">
+      <c r="U14" s="12">
         <v>-105.02010900000001</v>
       </c>
-      <c r="U14" s="24">
+      <c r="V14" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V14" s="25">
+      <c r="W14" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W14" s="25">
+      <c r="X14" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X14" s="22" t="s">
+      <c r="Y14" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="Y14" s="17">
+      <c r="Z14" s="17">
         <v>10</v>
       </c>
-      <c r="Z14" s="27">
+      <c r="AA14" s="27">
         <v>13119</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17">
         <v>13</v>
@@ -2174,98 +2228,102 @@
         <v>76</v>
       </c>
       <c r="H15" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="17">
+      <c r="J15" s="17">
         <v>4321</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="K15" s="18" t="s">
         <v>27</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="L15" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="19">
         <v>42369</v>
       </c>
-      <c r="N15" s="20">
+      <c r="O15" s="20">
         <v>482215</v>
       </c>
-      <c r="O15" s="21" t="s">
+      <c r="P15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="P15" s="17" t="s">
+      <c r="Q15" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Q15" s="21" t="s">
+      <c r="R15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="R15" s="17" t="s">
+      <c r="S15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="S15" s="12">
+      <c r="T15" s="12">
         <v>39.748420000000003</v>
       </c>
-      <c r="T15" s="12">
+      <c r="U15" s="12">
         <v>-105.007644</v>
       </c>
-      <c r="U15" s="24">
+      <c r="V15" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V15" s="25">
+      <c r="W15" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W15" s="25">
+      <c r="X15" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X15" s="22" t="s">
+      <c r="Y15" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="Y15" s="17">
+      <c r="Z15" s="17">
         <v>11</v>
       </c>
-      <c r="Z15" s="27">
+      <c r="AA15" s="27">
         <v>13150</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="E16"/>
     </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E17"/>
-      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E18"/>
-      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E19"/>
-      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E20"/>
-      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E21"/>
-      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E22"/>
-      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E23"/>
-      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W13">
     <sortCondition ref="B2:B13"/>
   </sortState>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="C2:D2 C9 C11 C5:D6 C7 F2:F13">
     <cfRule type="duplicateValues" dxfId="2" priority="97"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added leading zeros to 0 zip; modified test to do explicit check
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-postal.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-postal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761DD01B-22CE-284D-B228-A678603F2BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2F1869-B008-CE41-8D14-0851C2BBB2C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38560" yWindow="2000" windowWidth="38400" windowHeight="19640" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="1960" windowWidth="38400" windowHeight="19640" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -381,9 +381,6 @@
     <t>86HJX838+8M7-1-3-1-2</t>
   </si>
   <si>
-    <t>12345-6789</t>
-  </si>
-  <si>
     <t>1-2</t>
   </si>
   <si>
@@ -394,6 +391,12 @@
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>31-24</t>
+  </si>
+  <si>
+    <t>0-0</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1067,8 @@
   </sheetPr>
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1119,7 +1122,7 @@
         <v>83</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>47</v>
@@ -1176,7 +1179,7 @@
         <v>93</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1332,7 +1335,7 @@
         <v>4</v>
       </c>
       <c r="AA3" s="28" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1731,7 +1734,7 @@
       <c r="Z8" s="7">
         <v>10</v>
       </c>
-      <c r="AA8" s="27" t="s">
+      <c r="AA8" s="28" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1753,10 +1756,10 @@
         <v>23</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>48</v>
@@ -1812,8 +1815,8 @@
       <c r="Z9" s="7">
         <v>11</v>
       </c>
-      <c r="AA9" s="27">
-        <v>0</v>
+      <c r="AA9" s="27" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Release for 2.17.0 (#3721)
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-postal.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-postal.xlsx
@@ -1,30 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D3E00C-3725-AE45-8E28-B0CD0CFB5BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E521081D-DCAA-9C46-BFBC-C805CF60705C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="17540" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -586,32 +618,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -627,13 +650,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="94">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1065,42 +1087,40 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="8.83203125" style="12"/>
-    <col min="22" max="22" width="12.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11" style="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="8.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.83203125" style="12"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1163,7 +1183,7 @@
       <c r="U1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -1172,1155 +1192,1117 @@
       <c r="X1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="1" t="s">
         <v>93</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="5">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2">
         <v>2264</v>
       </c>
-      <c r="D2" s="6"/>
       <c r="E2" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2">
         <v>1552813</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2">
         <v>75</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2">
         <v>125</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="4">
         <v>42369</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="5">
         <v>12555</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2">
         <v>39.755543000000003</v>
       </c>
-      <c r="U2" s="5">
+      <c r="U2">
         <v>-105.22110000000001</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="W2" s="25">
+      <c r="W2" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X2" s="25">
+      <c r="X2" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Z2" s="7">
+      <c r="Z2">
         <v>1</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B3">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3">
         <v>1154623</v>
       </c>
-      <c r="D3" s="6"/>
       <c r="E3" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3">
         <v>11160509</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3">
         <v>63</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3">
         <v>1202</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="4">
         <v>42369</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="5">
         <v>23543</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" t="s">
         <v>45</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3">
         <v>39.751511000000001</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3">
         <v>-105.225381</v>
       </c>
-      <c r="V3" s="24">
+      <c r="V3" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W3" s="25">
+      <c r="W3" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="Z3" s="7">
+      <c r="Z3">
         <v>4</v>
       </c>
-      <c r="AA3" s="28" t="s">
+      <c r="AA3" s="20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="5">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <v>1311523</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>1311523</v>
       </c>
       <c r="E4" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4">
         <v>24651456</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="4">
         <v>42369</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" t="s">
         <v>26</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4">
         <v>39.740510999999998</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4">
         <v>-105.17121</v>
       </c>
-      <c r="V4" s="24"/>
-      <c r="W4" s="25">
+      <c r="V4" s="17"/>
+      <c r="W4" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X4" s="25">
+      <c r="X4" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y4" s="9" t="s">
+      <c r="Y4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="Z4">
         <v>6</v>
       </c>
-      <c r="AA4" s="27">
+      <c r="AA4" s="19">
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="5">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B5">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5">
         <v>1311524</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>1311523</v>
       </c>
       <c r="E5" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5">
         <v>24651456</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5">
         <v>77</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5">
         <v>219</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="4">
         <v>42369</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="8">
         <v>124523</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5">
         <v>39.734164</v>
       </c>
-      <c r="U5" s="5">
+      <c r="U5">
         <v>-105.159808</v>
       </c>
-      <c r="V5" s="24">
+      <c r="V5" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W5" s="25">
+      <c r="W5" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Y5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="Z5">
         <v>7</v>
       </c>
-      <c r="AA5" s="27">
+      <c r="AA5" s="19">
         <v>88051</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B6">
         <v>11</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>1311525</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>1311523</v>
       </c>
       <c r="E6" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6">
         <v>24651456</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6">
         <v>43</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6">
         <v>84</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="4">
         <v>42369</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="8">
         <v>421351</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6">
         <v>39.733597000000003</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6">
         <v>-105.162576</v>
       </c>
-      <c r="V6" s="24">
+      <c r="V6" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W6" s="25">
+      <c r="W6" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X6" s="25">
+      <c r="X6" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Y6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="Z6">
         <v>8</v>
       </c>
-      <c r="AA6" s="27">
+      <c r="AA6" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <v>1311526</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7">
         <v>1311523</v>
       </c>
       <c r="E7" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7">
         <v>24651456</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7">
         <v>59</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7">
         <v>72</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="4">
         <v>42369</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="8">
         <v>1234</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="P7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="R7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="S7" t="s">
         <v>26</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7">
         <v>39.739111000000001</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7">
         <v>-104.984951</v>
       </c>
-      <c r="V7" s="24">
+      <c r="V7" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W7" s="25">
+      <c r="W7" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X7" s="25">
+      <c r="X7" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y7" s="9" t="s">
+      <c r="Y7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="Z7">
         <v>9</v>
       </c>
-      <c r="AA7" s="27">
+      <c r="AA7" s="19">
         <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>9</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8">
         <v>1311527</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <v>1311523</v>
       </c>
       <c r="E8" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8">
         <v>34</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8">
         <v>45</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="4">
         <v>42369</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="8">
         <v>45324</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="P8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" t="s">
         <v>40</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="R8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="S8" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="12">
+      <c r="T8">
         <v>39.731361</v>
       </c>
-      <c r="U8" s="12">
+      <c r="U8">
         <v>-104.96074299999999</v>
       </c>
-      <c r="V8" s="24">
+      <c r="V8" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W8" s="25">
+      <c r="W8" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X8" s="25">
+      <c r="X8" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y8" s="9" t="s">
+      <c r="Y8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="Z8">
         <v>10</v>
       </c>
-      <c r="AA8" s="28" t="s">
+      <c r="AA8" s="20" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>12</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>1311528</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <v>1311523</v>
       </c>
       <c r="E9" t="s">
         <v>110</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" t="s">
         <v>119</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" t="s">
         <v>119</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="4">
         <v>42369</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="8">
         <v>482215</v>
       </c>
-      <c r="P9" s="11" t="s">
+      <c r="P9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="Q9" t="s">
         <v>40</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="R9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="S9" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="12">
+      <c r="T9">
         <v>39.741906999999998</v>
       </c>
-      <c r="U9" s="12">
+      <c r="U9">
         <v>-104.975129</v>
       </c>
-      <c r="V9" s="24">
+      <c r="V9" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W9" s="25">
+      <c r="W9" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X9" s="25">
+      <c r="X9" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y9" s="9" t="s">
+      <c r="Y9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9">
         <v>11</v>
       </c>
-      <c r="AA9" s="27" t="s">
+      <c r="AA9" s="19" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10">
         <v>3020139</v>
       </c>
-      <c r="D10" s="5"/>
       <c r="E10" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10">
         <v>11160509</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10">
         <v>1</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10">
         <v>652.29999999999995</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="4">
         <v>42369</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="5">
         <v>513852</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="Q10" t="s">
         <v>45</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="R10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="S10" t="s">
         <v>15</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10">
         <v>39.742130000000003</v>
       </c>
-      <c r="U10" s="12">
+      <c r="U10">
         <v>-104.996673</v>
       </c>
-      <c r="V10" s="24">
+      <c r="V10" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W10" s="25">
+      <c r="W10" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X10" s="25">
+      <c r="X10" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y10" s="9" t="s">
+      <c r="Y10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="Z10">
         <v>2</v>
       </c>
-      <c r="AA10" s="27">
+      <c r="AA10" s="19">
         <v>80504</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11">
         <v>4828379</v>
       </c>
-      <c r="D11" s="5"/>
       <c r="E11" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11">
         <v>11160509</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="4">
         <v>42369</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="5">
         <v>55121</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="P11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="Q11" t="s">
         <v>45</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="R11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="7" t="s">
+      <c r="S11" t="s">
         <v>15</v>
       </c>
-      <c r="T11" s="12">
+      <c r="T11">
         <v>40.014986</v>
       </c>
-      <c r="U11" s="12">
+      <c r="U11">
         <v>-105.270546</v>
       </c>
-      <c r="V11" s="24">
+      <c r="V11" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W11" s="25">
+      <c r="W11" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X11" s="25">
+      <c r="X11" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y11" s="9" t="s">
+      <c r="Y11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z11">
         <v>3</v>
       </c>
-      <c r="AA11" s="27">
+      <c r="AA11" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5">
+      <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12">
         <v>5233255</v>
       </c>
-      <c r="D12" s="6"/>
       <c r="E12" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" t="s">
         <v>78</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12">
         <v>55</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12">
         <v>1358</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="4">
         <v>42369</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="5">
         <v>200000</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="P12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="Q12" t="s">
         <v>46</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="R12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S12" s="7" t="s">
+      <c r="S12" t="s">
         <v>16</v>
       </c>
-      <c r="T12" s="12">
+      <c r="T12">
         <v>40.007199</v>
       </c>
-      <c r="U12" s="12">
+      <c r="U12">
         <v>-105.26486800000001</v>
       </c>
-      <c r="V12" s="24">
+      <c r="V12" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W12" s="25">
+      <c r="W12" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X12" s="25">
+      <c r="X12" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y12" s="9" t="s">
+      <c r="Y12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="Z12">
         <v>5</v>
       </c>
-      <c r="AA12" s="27">
-        <v>3</v>
+      <c r="AA12" s="19" t="e" cm="1">
+        <f t="array" ref="AA12">abc/2</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B13" s="5">
+      <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13">
         <v>6798215</v>
       </c>
       <c r="E13" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13">
         <v>13334485</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13">
         <v>88</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13">
         <v>942</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="4">
         <v>42369</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="9">
         <v>24523</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="P13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="12" t="s">
+      <c r="Q13" t="s">
         <v>56</v>
       </c>
-      <c r="R13" s="15" t="s">
+      <c r="R13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="S13" s="7" t="s">
+      <c r="S13" t="s">
         <v>58</v>
       </c>
-      <c r="T13" s="12">
+      <c r="T13">
         <v>39.999355999999999</v>
       </c>
-      <c r="U13" s="12">
+      <c r="U13">
         <v>-105.26242000000001</v>
       </c>
-      <c r="V13" s="24">
+      <c r="V13" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W13" s="25">
+      <c r="W13" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X13" s="25">
+      <c r="X13" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y13" s="9" t="s">
+      <c r="Y13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="Z13">
         <v>12</v>
       </c>
-      <c r="AA13" s="27">
+      <c r="AA13" s="19">
         <v>13089</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10">
         <v>13</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="11">
         <v>481516</v>
       </c>
-      <c r="D14" s="17"/>
+      <c r="D14" s="10"/>
       <c r="E14" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="10">
         <v>1234</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="11">
         <v>34</v>
       </c>
-      <c r="M14" s="18">
-        <v>45</v>
-      </c>
-      <c r="N14" s="19">
+      <c r="M14" s="11" t="e">
+        <f>123/"abc"</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N14" s="12">
         <v>42369</v>
       </c>
-      <c r="O14" s="20">
+      <c r="O14" s="13">
         <v>45324</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q14" s="17" t="s">
+      <c r="Q14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="R14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="S14" s="17" t="s">
+      <c r="S14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="T14" s="12">
+      <c r="T14">
         <v>39.74389</v>
       </c>
-      <c r="U14" s="12">
+      <c r="U14">
         <v>-105.02010900000001</v>
       </c>
-      <c r="V14" s="24">
+      <c r="V14" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W14" s="25">
+      <c r="W14" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X14" s="25">
+      <c r="X14" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y14" s="22" t="s">
+      <c r="Y14" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="Z14" s="17">
+      <c r="Z14" s="10">
         <v>10</v>
       </c>
-      <c r="AA14" s="27">
-        <v>13119</v>
+      <c r="AA14" s="19" t="e">
+        <f>50/0</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10">
         <v>13</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="11">
         <v>2342</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="10"/>
       <c r="E15" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="10">
         <v>4321</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="17" t="s">
+      <c r="M15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="12">
         <v>42369</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="13">
         <v>482215</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q15" s="17" t="s">
+      <c r="Q15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="21" t="s">
+      <c r="R15" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="S15" s="17" t="s">
+      <c r="S15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="T15" s="12">
+      <c r="T15">
         <v>39.748420000000003</v>
       </c>
-      <c r="U15" s="12">
+      <c r="U15">
         <v>-105.007644</v>
       </c>
-      <c r="V15" s="24">
+      <c r="V15" s="17">
         <v>42740.333333333336</v>
       </c>
-      <c r="W15" s="25">
+      <c r="W15" s="17">
         <v>42891.739583333336</v>
       </c>
-      <c r="X15" s="25">
+      <c r="X15" s="17">
         <v>42987.961805555555</v>
       </c>
-      <c r="Y15" s="22" t="s">
+      <c r="Y15" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="Z15" s="17">
+      <c r="Z15" s="10">
         <v>11</v>
       </c>
-      <c r="AA15" s="27">
-        <v>13150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="E16"/>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E17"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E18"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E19"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E20"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E21"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E22"/>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E23"/>
-      <c r="J23" s="5"/>
+      <c r="AA15" s="19" t="e">
+        <f>123/"abc"</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W13">

</xml_diff>